<commit_message>
init all application edited
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +79,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -159,13 +150,61 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>WI4_Items</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>Generate Yearly Report Performer</t>
+  </si>
+  <si>
+    <t>Report_DIR</t>
+  </si>
+  <si>
+    <t>Data\Report\</t>
+  </si>
+  <si>
+    <t>System1_Credential</t>
+  </si>
+  <si>
+    <t>System1Credential</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items</t>
+  </si>
+  <si>
+    <t>System1WorkITemsURL</t>
+  </si>
+  <si>
+    <t>DownloadMonthlyReportsURL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/reports/download</t>
+  </si>
+  <si>
+    <t>UploadYearlyReportURL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/reports/upload</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
+  </si>
+  <si>
+    <t>System1LoginURL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -211,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -221,6 +260,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -281,7 +322,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -333,7 +374,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -527,18 +568,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -585,42 +626,93 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
-      <c r="A5" t="s">
+    <row r="4" spans="1:26" ht="28.8">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
+      <c r="B4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1616,7 +1708,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1673,18 +1765,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1800,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1822,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1833,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1844,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2779,10 +2871,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2800,7 +2892,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>